<commit_message>
Import Excel data to asset table
</commit_message>
<xml_diff>
--- a/TechEngineer/src/TechEngineer.Web.Mvc/wwwroot/excel/TechEngineerAssetsSample.xlsx
+++ b/TechEngineer/src/TechEngineer.Web.Mvc/wwwroot/excel/TechEngineerAssetsSample.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Inside\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\proj\TechEngineerGit\TechEngineer\src\TechEngineer.Web.Mvc\wwwroot\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="945" yWindow="0" windowWidth="3795" windowHeight="6600"/>
+    <workbookView xWindow="1890" yWindow="0" windowWidth="3795" windowHeight="6600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t>[assetId]</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>[Name]</t>
   </si>
@@ -35,61 +32,115 @@
     <t>[Category]</t>
   </si>
   <si>
-    <t>[Serial Number]</t>
-  </si>
-  <si>
     <t>[Department]</t>
   </si>
   <si>
     <t>[IPAddress]</t>
   </si>
   <si>
-    <t>[System username]</t>
-  </si>
-  <si>
     <t>[CPU]</t>
   </si>
   <si>
-    <t>[Mother board]</t>
-  </si>
-  <si>
     <t>[RAM]</t>
   </si>
   <si>
     <t>[HDD]</t>
   </si>
   <si>
-    <t>[Monitor]</t>
-  </si>
-  <si>
-    <t>[Monitor_Serial no]</t>
-  </si>
-  <si>
-    <t>[Key board]</t>
-  </si>
-  <si>
     <t>[Mouse]</t>
   </si>
   <si>
-    <t>[Operating system]</t>
-  </si>
-  <si>
-    <t>[MSOffice]</t>
-  </si>
-  <si>
-    <t>[Purchase date]</t>
-  </si>
-  <si>
     <t>[Details]</t>
   </si>
   <si>
-    <t>[Model number]</t>
-  </si>
-  <si>
-    <t>[Is in warrenty]</t>
-  </si>
-  <si>
-    <t>[Is active]</t>
+    <t>[Id]</t>
+  </si>
+  <si>
+    <t>[SerialNumber]</t>
+  </si>
+  <si>
+    <t>[ModelNumber]</t>
+  </si>
+  <si>
+    <t>[IsActive]</t>
+  </si>
+  <si>
+    <t>[IsinWarrenty]</t>
+  </si>
+  <si>
+    <t>[OrganizationId]</t>
+  </si>
+  <si>
+    <t>[LocationId]</t>
+  </si>
+  <si>
+    <t>[CreationTime]</t>
+  </si>
+  <si>
+    <t>[CreatorUserId]</t>
+  </si>
+  <si>
+    <t>[KeyBoard]</t>
+  </si>
+  <si>
+    <t>[OperatingSystem]</t>
+  </si>
+  <si>
+    <t>[PurchaseDate]</t>
+  </si>
+  <si>
+    <t>[System_Username]</t>
+  </si>
+  <si>
+    <t>3041473f-0a49-4c3c-8e9c-5d23885528b1</t>
+  </si>
+  <si>
+    <t>Machine103</t>
+  </si>
+  <si>
+    <t>Test Details</t>
+  </si>
+  <si>
+    <t>Test Category</t>
+  </si>
+  <si>
+    <t>S10254789</t>
+  </si>
+  <si>
+    <t>Model10254302</t>
+  </si>
+  <si>
+    <t>3B613A6C-3CA8-4180-46C4-08DA812F87EE</t>
+  </si>
+  <si>
+    <t>FD8714C0-854E-4A34-4EF5-08DA812F8808</t>
+  </si>
+  <si>
+    <t>CPU</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>2GB DDR</t>
+  </si>
+  <si>
+    <t>124.3.36.520</t>
+  </si>
+  <si>
+    <t>Lenovo</t>
+  </si>
+  <si>
+    <t>Dell</t>
+  </si>
+  <si>
+    <t>Windows10</t>
+  </si>
+  <si>
+    <t>8GB</t>
+  </si>
+  <si>
+    <t>Roma Soni</t>
   </si>
 </sst>
 </file>
@@ -125,8 +176,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,98 +459,171 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.28515625" customWidth="1"/>
+    <col min="10" max="10" width="37.42578125" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" customWidth="1"/>
+    <col min="15" max="15" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.42578125" customWidth="1"/>
+    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.140625" customWidth="1"/>
+    <col min="20" max="20" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="O1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="Q1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
       </c>
       <c r="V1" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="1">
+        <v>44686</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" s="1">
+        <v>44783</v>
+      </c>
+      <c r="U2" t="s">
+        <v>37</v>
+      </c>
+      <c r="V2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>